<commit_message>
Update DateBase/orders/Dang Nguyen 195_2025-12-31.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Dang Nguyen 195_2025-12-31.xlsx
+++ b/DateBase/orders/Dang Nguyen 195_2025-12-31.xlsx
@@ -523,6 +523,9 @@
       <c r="C11" t="str">
         <v>221_朱丽叶塔_Julieta_Rosa rugosa Thunb._10stems</v>
       </c>
+      <c r="F11" t="str">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -584,7 +587,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>014613710139870</v>
+        <v>014613710139878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>